<commit_message>
continue to update files for all-spreadsheet inputs
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -732,14 +732,14 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="X63" activeCellId="0" sqref="X63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,7 +1154,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,7 +1224,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,12 +1302,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="R41" activeCellId="0" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.91836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,13 +1415,12 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="P46" activeCellId="0" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,13 +1748,12 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1939,14 +1945,14 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="L64" activeCellId="0" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,13 +2262,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
+      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2330,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2483,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,9 +2693,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,7 +2792,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,7 +2920,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2969,8 +2981,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update script docstrings, change eg_dict to p_dict
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
     <sheet name="ratio_cond" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="count_ratio_cond" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="quota_dict" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="eg_dictionary" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="proposal_dictionary" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="eg_colors" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="basic_job_colors" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="enhanced_job_colors" sheetId="14" state="visible" r:id="rId15"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="184">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t xml:space="preserve">cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proposal</t>
   </si>
   <si>
     <t xml:space="preserve">short_descr</t>
@@ -731,8 +734,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,8 +1134,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,25 +1198,25 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1283,8 +1287,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,19 +1296,19 @@
         <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,19 +1316,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,19 +1336,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,19 +1356,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1391,8 +1395,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,16 +1403,16 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,8 +1592,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,16 +1600,16 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,9 +1925,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,16 +2236,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2302,6 +2304,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2453,8 +2458,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,10 +2668,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2762,8 +2767,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,8 +2895,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,9 +2956,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add count_ratio_dict worksheet to settings.xlsx, modify function make_lists_from_columns, delete function make_intlists_from_columns, add count_ratio_dict basic to enhanced conversion to convert function, add count_ratio_dict to build_program_files script >> all in prep for updating ratio count condition processing
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,10 +18,11 @@
     <sheet name="ratio_cond" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="count_ratio_cond" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="quota_dict" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="proposal_dictionary" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="eg_colors" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="basic_job_colors" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="enhanced_job_colors" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="count_ratio_dict" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="proposal_dictionary" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="eg_colors" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="basic_job_colors" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="enhanced_job_colors" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="192">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -498,6 +499,30 @@
   </si>
   <si>
     <t xml:space="preserve">cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, 3 </t>
   </si>
   <si>
     <t xml:space="preserve">proposal</t>
@@ -734,9 +759,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,8 +1159,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,71 +1221,114 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>157</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>159</v>
+      <c r="E2" s="7" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>320</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>162</v>
+      <c r="E3" s="7" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>580</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1279,96 +1347,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>173</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>179</v>
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1430,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1395,177 +1438,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>1</v>
+      <c r="B2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>1</v>
+      <c r="B3" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>0.94</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>1</v>
+      <c r="B4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1584,6 +1538,204 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1592,7 +1744,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,16 +1753,16 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,9 +2078,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.6632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,10 +2394,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2457,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,8 +2610,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,10 +2820,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,8 +2919,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2895,8 +3047,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,9 +3108,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor assign_cond_ratio_capped and assign_jobs_nbnf_job_changes functions to permit a full range of inputs - any ratio grouping of employee groups for any job for any time period.  update build_program_files script to sync with above changes and to produce sets of month ranges for various conditional assignment routines
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="189">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -417,10 +417,7 @@
     <t xml:space="preserve">change</t>
   </si>
   <si>
-    <t xml:space="preserve">start_month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_month</t>
+    <t xml:space="preserve">month_end</t>
   </si>
   <si>
     <t xml:space="preserve">total_change</t>
@@ -517,12 +514,6 @@
   </si>
   <si>
     <t xml:space="preserve">weight3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">month_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2, 3 </t>
   </si>
   <si>
     <t xml:space="preserve">proposal</t>
@@ -754,14 +745,14 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,8 +1150,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,13 +1158,13 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,47 +1214,47 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>120</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,8 +1264,8 @@
       <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>162</v>
+      <c r="C2" s="7" t="n">
+        <v>2</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>0</v>
@@ -1310,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>2.46</v>
@@ -1319,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>580</v>
@@ -1355,19 +1345,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,10 +1364,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,7 +1389,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1438,8 +1427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,19 +1435,19 @@
         <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,19 +1455,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,19 +1475,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,19 +1495,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1546,8 +1534,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,16 +1543,16 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,8 +1732,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,16 +1741,16 @@
         <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,8 +2066,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,10 +2383,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2444,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,13 +2592,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z26" activeCellId="0" sqref="Z26"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2622,13 +2608,13 @@
         <v>122</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>123</v>
@@ -2642,7 +2628,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2668,7 +2654,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>4</v>
@@ -2694,7 +2680,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>2</v>
@@ -2720,7 +2706,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>5</v>
@@ -2746,7 +2732,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
@@ -2772,7 +2758,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>6</v>
@@ -2815,15 +2801,14 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,7 +2816,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>123</v>
@@ -2843,15 +2828,15 @@
         <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>8</v>
@@ -2874,7 +2859,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>10</v>
@@ -2914,18 +2899,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>66</v>
@@ -2934,18 +2918,18 @@
         <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2965,7 +2949,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -2985,7 +2969,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1</v>
@@ -3005,7 +2989,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
@@ -3039,49 +3023,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>1</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="7" t="n">
         <v>4</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3108,28 +3111,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>2</v>
@@ -3143,7 +3145,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
delete quota_dict and count_ratio_condition worksheets in settings.xlsx input file, remove code to store related data in the settings dictionary.
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,11 @@
     <sheet name="recall" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="prex" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="ratio_cond" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="count_ratio_cond" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="quota_dict" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="count_ratio_dict" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="proposal_dictionary" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="eg_colors" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="basic_job_colors" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="enhanced_job_colors" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="ratio_count_capped_cond" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="proposal_dictionary" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="eg_colors" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="basic_job_colors" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="enhanced_job_colors" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="183">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -132,9 +130,6 @@
     <t xml:space="preserve">ratio_cond_duration</t>
   </si>
   <si>
-    <t xml:space="preserve">count_cond_duration</t>
-  </si>
-  <si>
     <t xml:space="preserve">sg_dist</t>
   </si>
   <si>
@@ -480,40 +475,25 @@
     <t xml:space="preserve">r2</t>
   </si>
   <si>
-    <t xml:space="preserve">count_ratio_cond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight_2</t>
+    <t xml:space="preserve">group1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight3</t>
   </si>
   <si>
     <t xml:space="preserve">cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight3</t>
   </si>
   <si>
     <t xml:space="preserve">proposal</t>
@@ -742,17 +722,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,27 +976,27 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="6" t="n">
-        <v>60</v>
+      <c r="B30" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,15 +1004,16 @@
         <v>37</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>36</v>
+      <c r="B34" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,15 +1093,6 @@
         <v>47</v>
       </c>
       <c r="B43" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1142,57 +1113,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>320</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>4</v>
+      <c r="A3" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>2.46</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>580</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1211,114 +1196,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="B2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="J2" s="6" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>2.46</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>580</v>
-      </c>
-      <c r="I3" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="J3" s="6" t="n">
-        <v>55</v>
+      <c r="B3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1337,70 +1304,186 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>162</v>
+        <v>180</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>164</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>165</v>
+        <v>0.14</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>166</v>
+        <v>0.66</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>167</v>
+        <v>0.28</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1419,311 +1502,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.2857142857143"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>0.94</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1732,25 +1510,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,297 +1844,297 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2383,19 +2161,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,22 +2223,19 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2597,38 +2374,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2654,7 +2432,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>4</v>
@@ -2680,7 +2458,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>2</v>
@@ -2706,7 +2484,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>5</v>
@@ -2732,7 +2510,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
@@ -2758,7 +2536,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>6</v>
@@ -2806,9 +2584,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,27 +2595,27 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>8</v>
@@ -2859,7 +2638,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>10</v>
@@ -2904,32 +2683,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2949,7 +2729,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -2969,7 +2749,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1</v>
@@ -2989,7 +2769,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
@@ -3031,31 +2811,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -3072,7 +2853,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -3103,58 +2884,113 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>139</v>
+        <v>149</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>149</v>
+      <c r="A2" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>1</v>
-      </c>
       <c r="D2" s="7" t="n">
-        <v>92</v>
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>320</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="7" t="n">
+      <c r="A3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>168</v>
+      <c r="D3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>580</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify ratio condition job assignment routine and all related code to permit universal application with any combination of jobs and employee groups within the ratio groups, add pprint_dict function, modify settings.xlsx file for new ratio condition handling
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="179">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -127,9 +127,6 @@
     <t xml:space="preserve">ret_age_increase</t>
   </si>
   <si>
-    <t xml:space="preserve">ratio_cond_duration</t>
-  </si>
-  <si>
     <t xml:space="preserve">sg_dist</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t xml:space="preserve">count_dist</t>
   </si>
   <si>
-    <t xml:space="preserve">quota_dist</t>
-  </si>
-  <si>
     <t xml:space="preserve">compute_job_category_order</t>
   </si>
   <si>
@@ -463,31 +457,25 @@
     <t xml:space="preserve">prex4</t>
   </si>
   <si>
-    <t xml:space="preserve">ratio_cond</t>
-  </si>
-  <si>
     <t xml:space="preserve">basic_job</t>
   </si>
   <si>
-    <t xml:space="preserve">r1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r2</t>
-  </si>
-  <si>
     <t xml:space="preserve">group1</t>
   </si>
   <si>
     <t xml:space="preserve">group2</t>
   </si>
   <si>
+    <t xml:space="preserve">weight1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">group3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight2</t>
   </si>
   <si>
     <t xml:space="preserve">weight3</t>
@@ -722,16 +710,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,43 +956,45 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="6" t="n">
-        <v>39</v>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>35</v>
+      <c r="B32" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>35</v>
+      <c r="B33" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,24 +1065,6 @@
         <v>45</v>
       </c>
       <c r="B41" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1121,19 +1093,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1204,28 +1176,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,19 +1205,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,19 +1225,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,19 +1245,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1312,25 +1284,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,25 +1482,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,297 +1816,297 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2162,20 +2134,20 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,16 +2198,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,39 +2346,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2432,7 +2404,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>4</v>
@@ -2458,7 +2430,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>2</v>
@@ -2484,7 +2456,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>5</v>
@@ -2510,7 +2482,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
@@ -2536,7 +2508,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>6</v>
@@ -2584,9 +2556,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -2595,27 +2567,27 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>8</v>
@@ -2638,7 +2610,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>10</v>
@@ -2683,33 +2655,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -2729,7 +2701,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -2749,7 +2721,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1</v>
@@ -2769,7 +2741,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
@@ -2803,69 +2775,86 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>126</v>
+        <v>145</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>145</v>
+      <c r="A2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="n">
+      <c r="C2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="n">
-        <v>73</v>
+      <c r="G2" s="6" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="7" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="E3" s="6" t="n">
-        <v>73</v>
+      <c r="G3" s="6" t="n">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2887,50 +2876,50 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
@@ -2952,13 +2941,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="7" t="n">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I2" s="6" t="n">
         <v>34</v>
       </c>
       <c r="J2" s="6" t="n">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,7 +2979,7 @@
         <v>34</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shorten lnum and lspcnt descriptions in attribute_dict worksheetof settings.xlsx input file for practical use in chart titles, remove all "example_chart" options from plotting functions, add exception types to most try/except blocks in plotting functions
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -325,13 +325,13 @@
     <t xml:space="preserve">lnum</t>
   </si>
   <si>
-    <t xml:space="preserve">list number (includes furloughed employees)</t>
+    <t xml:space="preserve">list number (includes fur)</t>
   </si>
   <si>
     <t xml:space="preserve">lspcnt</t>
   </si>
   <si>
-    <t xml:space="preserve">list percentage (includes furloughed employees)</t>
+    <t xml:space="preserve">list percent (includes fur)</t>
   </si>
   <si>
     <t xml:space="preserve">rank_in_job</t>
@@ -713,13 +713,14 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="P53" activeCellId="0" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,8 +1094,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,8 +1177,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1284,8 +1285,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,8 +1483,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,15 +1811,14 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,10 +2133,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,6 +2195,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2346,8 +2349,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,10 +2559,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2655,8 +2658,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,14 +2781,15 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,15 +2879,16 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor contract_year_and_raise function, remove items from settings dictionary that are no longer used, add pay_exceptions worksheet to settings.xlsx input file - this allows any number of pay exceptions for any length of time, update make_skeleton script to use the modified contract_year_and_raise function
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="attribute_dict" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ret_incr" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="job_counts" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="job_changes" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="recall" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="prex" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="ratio_cond" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="ratio_count_capped_cond" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="proposal_dictionary" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="eg_colors" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="basic_job_colors" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="enhanced_job_colors" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="pay_exceptions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="job_counts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="job_changes" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="recall" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="prex" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ratio_cond" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="ratio_count_capped_cond" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="proposal_dictionary" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="eg_colors" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="basic_job_colors" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="enhanced_job_colors" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="163">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -100,18 +101,6 @@
     <t xml:space="preserve">top_of_scale</t>
   </si>
   <si>
-    <t xml:space="preserve">pay_table_exception_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_exception_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_exception_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_contract_year</t>
-  </si>
-  <si>
     <t xml:space="preserve">pay_table_year_sort</t>
   </si>
   <si>
@@ -127,19 +116,19 @@
     <t xml:space="preserve">ret_age_increase</t>
   </si>
   <si>
-    <t xml:space="preserve">sg_dist</t>
+    <t xml:space="preserve">dist_sg</t>
   </si>
   <si>
     <t xml:space="preserve">part</t>
   </si>
   <si>
-    <t xml:space="preserve">ratio_dist</t>
+    <t xml:space="preserve">dist_ratio</t>
   </si>
   <si>
     <t xml:space="preserve">split</t>
   </si>
   <si>
-    <t xml:space="preserve">count_dist</t>
+    <t xml:space="preserve">dist_count</t>
   </si>
   <si>
     <t xml:space="preserve">compute_job_category_order</t>
@@ -382,15 +371,21 @@
     <t xml:space="preserve">cumulative career pay</t>
   </si>
   <si>
-    <t xml:space="preserve">increase</t>
-  </si>
-  <si>
     <t xml:space="preserve">month_start</t>
   </si>
   <si>
     <t xml:space="preserve">month_increase</t>
   </si>
   <si>
+    <t xml:space="preserve">year_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_date</t>
+  </si>
+  <si>
     <t xml:space="preserve">job</t>
   </si>
   <si>
@@ -403,58 +398,16 @@
     <t xml:space="preserve">eg3</t>
   </si>
   <si>
-    <t xml:space="preserve">change</t>
-  </si>
-  <si>
     <t xml:space="preserve">month_end</t>
   </si>
   <si>
     <t xml:space="preserve">total_change</t>
   </si>
   <si>
-    <t xml:space="preserve">jc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jc3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jc4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jc5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jc6</t>
-  </si>
-  <si>
     <t xml:space="preserve">total_monthly</t>
   </si>
   <si>
-    <t xml:space="preserve">recall1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recall2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prex_cond</t>
-  </si>
-  <si>
     <t xml:space="preserve">count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prex1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prex2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prex3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prex4</t>
   </si>
   <si>
     <t xml:space="preserve">basic_job</t>
@@ -710,17 +663,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P53" activeCellId="0" sqref="P53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +747,6 @@
         <v>11</v>
       </c>
       <c r="B9" s="5" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -888,23 +840,23 @@
         <v>22</v>
       </c>
       <c r="B20" s="7" t="n">
-        <v>2014.1</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="8" t="n">
-        <v>42004</v>
+      <c r="B21" s="7" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8" t="n">
-        <v>42004</v>
+      <c r="B22" s="7" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,72 +864,75 @@
         <v>25</v>
       </c>
       <c r="B23" s="7" t="n">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7" t="n">
-        <v>2018</v>
+      <c r="B24" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7" t="n">
-        <v>7</v>
+      <c r="B25" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="7" t="n">
-        <v>65</v>
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="7" t="n">
-        <v>0</v>
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>32</v>
+      <c r="A29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B30" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>34</v>
+      <c r="B31" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,42 +985,6 @@
         <v>41</v>
       </c>
       <c r="B37" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1086,71 +1005,114 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>154</v>
+      <c r="E2" s="7" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>318</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>157</v>
+      <c r="D3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>580</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1169,96 +1131,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>168</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>174</v>
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1214,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1285,178 +1222,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>178</v>
+        <v>145</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>1</v>
+      <c r="B2" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>1</v>
+      <c r="B3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>0.94</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>1</v>
+      <c r="B4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1475,6 +1322,203 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1483,25 +1527,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,302 +1854,303 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2125,50 +2169,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="n">
+      <c r="A2" s="8" t="n">
         <v>43131</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="B2" s="7" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="n">
+      <c r="A3" s="8" t="n">
         <v>43861</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="B3" s="7" t="n">
         <v>12</v>
       </c>
     </row>
@@ -2188,141 +2222,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>197</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>80</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>470</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>85</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>1056</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>443</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>412</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>163</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>628</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>96</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>1121</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>464</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>66</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0</v>
+      <c r="A2" s="6" t="n">
+        <v>2014.1</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>42004</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>42004</v>
       </c>
     </row>
   </sheetData>
@@ -2341,198 +2272,141 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>126</v>
+      <c r="A2" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>64</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>43</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>470</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="B4" s="7" t="n">
+        <v>1056</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>443</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>412</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>163</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>64</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>72</v>
-      </c>
-      <c r="F3" s="7" t="n">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>628</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>96</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>1121</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>464</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>54</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="G3" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" s="7" t="n">
+      <c r="D9" s="7" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>52</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>-408</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>-377</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>-23</v>
-      </c>
-      <c r="H4" s="7" t="n">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>52</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>-510</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>-474</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>-26</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>61</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>411</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>376</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>26</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>61</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>411</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>376</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>26</v>
-      </c>
-      <c r="H7" s="7" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2551,87 +2425,180 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>133</v>
+      <c r="A2" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>43</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>72</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>66</v>
+      </c>
+      <c r="F3" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="G3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="n">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>75</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>150</v>
+      <c r="B4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>52</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>-408</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>-377</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>-23</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>-510</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>-474</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>-26</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>61</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>411</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>376</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>61</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>411</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>376</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2650,116 +2617,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>137</v>
+      <c r="A2" s="7" t="n">
+        <v>8</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>43</v>
-      </c>
       <c r="E2" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>3</v>
-      </c>
       <c r="D3" s="7" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>43</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>130</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>67</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2778,87 +2706,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>146</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>43</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="G2" s="6" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>146</v>
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>130</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>2.46</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="G3" s="6" t="n">
-        <v>72</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>43</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>130</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2877,50 +2819,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,29 +2863,20 @@
       <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>2</v>
+      <c r="C2" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="n">
-        <v>318</v>
-      </c>
-      <c r="I2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="J2" s="6" t="n">
-        <v>94</v>
+      <c r="G2" s="6" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,29 +2886,20 @@
       <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>0</v>
+      <c r="C3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>2.46</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>2.46</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>580</v>
-      </c>
-      <c r="I3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="J3" s="6" t="n">
-        <v>94</v>
+      <c r="G3" s="6" t="n">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove old version of the editor tool and supporting functions
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -666,14 +666,13 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,7 +737,6 @@
         <v>10</v>
       </c>
       <c r="B8" s="5" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -1013,10 +1011,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,8 +1135,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,8 +1217,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,7 +1325,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1523,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,14 +1852,14 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,14 +2169,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,8 +2227,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,9 +2276,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2428,16 +2422,16 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="Q35" activeCellId="0" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,14 +2614,16 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,13 +2705,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2827,10 +2825,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor ratio and count_ratio conditional job assignment routines, add ratio capture capability (snapshot), add code to build_program_files script to support changes
</commit_message>
<xml_diff>
--- a/seniority_list/excel/sample3/settings.xlsx
+++ b/seniority_list/excel/sample3/settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="scalars" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="164">
   <si>
     <t xml:space="preserve">option</t>
   </si>
@@ -419,19 +419,22 @@
     <t xml:space="preserve">group2</t>
   </si>
   <si>
+    <t xml:space="preserve">group3</t>
+  </si>
+  <si>
     <t xml:space="preserve">weight1</t>
   </si>
   <si>
     <t xml:space="preserve">weight2</t>
   </si>
   <si>
+    <t xml:space="preserve">weight3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snapshot</t>
+  </si>
+  <si>
     <t xml:space="preserve">2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight3</t>
   </si>
   <si>
     <t xml:space="preserve">cap</t>
@@ -605,7 +608,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -646,6 +649,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -665,14 +672,15 @@
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,16 +1011,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,19 +1037,19 @@
         <v>127</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>112</v>
@@ -1046,6 +1057,9 @@
       <c r="J1" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -1077,6 +1091,10 @@
       </c>
       <c r="J2" s="6" t="n">
         <v>94</v>
+      </c>
+      <c r="K2" s="10" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,6 +1127,10 @@
       </c>
       <c r="J3" s="6" t="n">
         <v>94</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1135,18 +1157,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,10 +1176,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1217,8 +1239,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,19 +1248,19 @@
         <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,19 +1268,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,19 +1288,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,19 +1308,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1325,8 +1347,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,16 +1356,16 @@
         <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,8 +1545,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,16 +1554,16 @@
         <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,9 +1879,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,9 +2195,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,8 +2248,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,6 +2297,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2427,11 +2451,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,11 +2643,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,10 +2734,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,16 +2841,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="7.68367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="6" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="9.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,10 +2875,19 @@
         <v>129</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>121</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2860,19 +2898,29 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <v>2.48</v>
       </c>
-      <c r="E2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="I2" s="6" t="n">
         <v>72</v>
+      </c>
+      <c r="J2" s="10" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,20 +2930,30 @@
       <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>2.46</v>
+      <c r="C3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>3</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="I3" s="6" t="n">
         <v>72</v>
+      </c>
+      <c r="J3" s="10" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>